<commit_message>
Updated data Cleaned up everything All data is now in a format we can use
</commit_message>
<xml_diff>
--- a/data/R2F IPIP.xlsx
+++ b/data/R2F IPIP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birgitp/Box/Rise 2 Flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90214296-76C7-EF43-89E0-2DD9B8C80DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF29B5E-8414-9A4E-B300-42561BA098A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="460" windowWidth="21880" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21880" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Av9!aEyp</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Folivora20</t>
   </si>
 </sst>
 </file>
@@ -474,11 +480,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2796,6 +2802,142 @@
         <v>2</v>
       </c>
     </row>
+    <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="6">
+        <v>44208.805103692124</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="6">
+        <v>44209.580218356481</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Cleanup - Added more plots - More explanations
</commit_message>
<xml_diff>
--- a/data/R2F IPIP.xlsx
+++ b/data/R2F IPIP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birgitp/Box/Rise 2 Flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF29B5E-8414-9A4E-B300-42561BA098A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055CCAF6-2BBB-494F-B907-FBB98D9AC5F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21880" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21880" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -70,15 +70,9 @@
     <t>V01vox</t>
   </si>
   <si>
-    <t>pclausen@grundfos.com</t>
-  </si>
-  <si>
     <t>Doughnut*7</t>
   </si>
   <si>
-    <t>mavipasi</t>
-  </si>
-  <si>
     <t>414Roseave!</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>faucar</t>
   </si>
   <si>
-    <t xml:space="preserve">Rakshita Anand </t>
-  </si>
-  <si>
     <t>Av9!aEyp</t>
   </si>
   <si>
@@ -203,6 +194,15 @@
   </si>
   <si>
     <t>Folivora20</t>
+  </si>
+  <si>
+    <t>pclau</t>
+  </si>
+  <si>
+    <t>Rakshita A</t>
+  </si>
+  <si>
+    <t>mavi</t>
   </si>
 </sst>
 </file>
@@ -222,6 +222,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -484,7 +485,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -497,67 +498,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1245,7 +1246,7 @@
         <v>44179.42281462963</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -1313,7 +1314,7 @@
         <v>44179.511538506944</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -1381,7 +1382,7 @@
         <v>44179.660243090279</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -1449,7 +1450,7 @@
         <v>44180.445999039352</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
@@ -1517,7 +1518,7 @@
         <v>44180.511878773148</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1585,7 +1586,7 @@
         <v>44180.701555925931</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -1653,7 +1654,7 @@
         <v>44181.919295162035</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
@@ -1721,7 +1722,7 @@
         <v>44187.732082719907</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>4</v>
@@ -1789,7 +1790,7 @@
         <v>44190.906370405093</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -1857,7 +1858,7 @@
         <v>44191.157136875001</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1925,7 +1926,7 @@
         <v>44198.732522361111</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
@@ -1991,7 +1992,7 @@
         <v>44201.568379108794</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -2059,7 +2060,7 @@
         <v>44201.621009803246</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -2127,7 +2128,7 @@
         <v>44201.647219467588</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -2195,7 +2196,7 @@
         <v>44201.684216597219</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
@@ -2263,7 +2264,7 @@
         <v>44201.709919918983</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -2331,7 +2332,7 @@
         <v>44201.723265023145</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>5</v>
@@ -2399,7 +2400,7 @@
         <v>44201.764723553242</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -2467,7 +2468,7 @@
         <v>44201.838143229164</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -2535,7 +2536,7 @@
         <v>44203.580405150467</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
@@ -2603,7 +2604,7 @@
         <v>44205.213217199074</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -2671,7 +2672,7 @@
         <v>44205.267144884259</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -2739,7 +2740,7 @@
         <v>44205.926264652779</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -2807,7 +2808,7 @@
         <v>44208.805103692124</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -2875,7 +2876,7 @@
         <v>44209.580218356481</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>

</xml_diff>